<commit_message>
Added a print statement for the routes
</commit_message>
<xml_diff>
--- a/datasheet_kopie.xlsx
+++ b/datasheet_kopie.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keesoosterhout/Documents/Documents - Kees’s MacBook Pro/TU Delft/MSc/Jaar 1/Q1/Operations Optimisation/Operations Assignment 2/MILP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanblackmore/Documents/AA Studie/Master/Q1/Operations Optimisation/MILP_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342595D7-BD1A-374C-8C9B-0C204D782267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19268DB-6941-184A-955E-F690FE7E2E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{5F5361A1-35E0-444D-99D6-775B076FC792}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" activeTab="2" xr2:uid="{5F5361A1-35E0-444D-99D6-775B076FC792}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="1" r:id="rId1"/>
-    <sheet name="Vertices" sheetId="3" r:id="rId2"/>
-    <sheet name="Arcs" sheetId="2" r:id="rId3"/>
+    <sheet name="NL_vertices" sheetId="3" r:id="rId2"/>
+    <sheet name="NL_arcs" sheetId="2" r:id="rId3"/>
     <sheet name="Other" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -298,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -931,7 +931,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
25 steden gemaakt ipv 49
</commit_message>
<xml_diff>
--- a/datasheet_kopie.xlsx
+++ b/datasheet_kopie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanblackmore/Documents/AA Studie/Master/Q1/Operations Optimisation/MILP_Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keesoosterhout/Documents/Documents - Kees’s MacBook Pro/TU Delft/MSc/Jaar 1/Q1/Operations Optimisation/Operations Assignment 2/MILP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4BE670-1713-1340-8FA0-788C8B198CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAA33C8-87D0-AA45-B7D3-EBA9A92D9329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{5F5361A1-35E0-444D-99D6-775B076FC792}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{5F5361A1-35E0-444D-99D6-775B076FC792}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="1" r:id="rId1"/>
@@ -300,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -314,10 +314,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -333,7 +332,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1128,7 +1127,7 @@
       <c r="D10" s="9">
         <v>6</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10">
         <v>12</v>
       </c>
     </row>
@@ -1145,7 +1144,7 @@
       <c r="D11" s="9">
         <v>11</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11">
         <v>22</v>
       </c>
     </row>
@@ -1162,7 +1161,7 @@
       <c r="D12" s="9">
         <v>14</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12">
         <v>28</v>
       </c>
     </row>
@@ -1179,7 +1178,7 @@
       <c r="D13" s="9">
         <v>12</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13">
         <v>24</v>
       </c>
     </row>
@@ -1283,7 +1282,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1307,10 +1306,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>100</v>

</xml_diff>